<commit_message>
Data is now linked
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Game</t>
   </si>
@@ -46,16 +46,44 @@
   </si>
   <si>
     <t>201210300CLE</t>
+  </si>
+  <si>
+    <t>201210300LAL</t>
+  </si>
+  <si>
+    <t>201210300MIA</t>
+  </si>
+  <si>
+    <t>201210310CHI</t>
+  </si>
+  <si>
+    <t>201210310DET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +106,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,15 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,14 +477,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -469,9 +505,133 @@
         <f>C2-D2</f>
         <v>1</v>
       </c>
+      <c r="H2">
+        <f>D2/MAX(B2:C2)*100</f>
+        <v>99.124726477024069</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>450</v>
+      </c>
+      <c r="C3">
+        <v>448</v>
+      </c>
+      <c r="D3">
+        <v>446</v>
+      </c>
+      <c r="E3">
+        <f>B3-D3</f>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>C3-D3</f>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f>D3/MAX(B3:C3)*100</f>
+        <v>99.111111111111114</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>421</v>
+      </c>
+      <c r="C4">
+        <v>422</v>
+      </c>
+      <c r="D4">
+        <v>421</v>
+      </c>
+      <c r="E4">
+        <f>B4-D4</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>C4-D4</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>D4/MAX(B4:C4)*100</f>
+        <v>99.76303317535546</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>480</v>
+      </c>
+      <c r="C5">
+        <v>478</v>
+      </c>
+      <c r="D5">
+        <v>476</v>
+      </c>
+      <c r="E5">
+        <f>B5-D5</f>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f>C5-D5</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f>D5/MAX(B5:C5)*100</f>
+        <v>99.166666666666671</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>432</v>
+      </c>
+      <c r="C6">
+        <v>430</v>
+      </c>
+      <c r="D6">
+        <v>427</v>
+      </c>
+      <c r="E6">
+        <f>B6-D6</f>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f>C6-D6</f>
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f>D6/MAX(B6:C6)*100</f>
+        <v>98.842592592592595</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>